<commit_message>
modificacion p0lantilla nuevo fonarte
</commit_message>
<xml_diff>
--- a/Videos (1).xlsx
+++ b/Videos (1).xlsx
@@ -3867,7 +3867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3885,11 +3885,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4311,8 +4306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119:XFD119"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4357,187 +4352,187 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>765</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>766</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>518</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>386</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="13" t="s">
         <v>388</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>767</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>768</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>519</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>386</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>769</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>770</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="12" t="s">
         <v>520</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>771</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>772</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
         <v>521</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="13" t="s">
         <v>394</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>773</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>774</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>522</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>775</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>776</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="13">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>777</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>778</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="12" t="s">
         <v>524</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="13" t="s">
         <v>492</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="13" t="s">
         <v>493</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="13">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>779</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>780</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="12" t="s">
         <v>525</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="13" t="s">
         <v>495</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="13">
         <v>8</v>
       </c>
     </row>
@@ -4564,1245 +4559,1245 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>783</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>784</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="13" t="s">
         <v>499</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="13">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>785</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>786</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="12" t="s">
         <v>528</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="13" t="s">
         <v>500</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="13">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>787</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>788</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="12" t="s">
         <v>529</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="13" t="s">
         <v>503</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="13" t="s">
         <v>502</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>789</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="12" t="s">
         <v>790</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="13" t="s">
         <v>504</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="13" t="s">
         <v>505</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="13">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>791</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>792</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="12" t="s">
         <v>531</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="13" t="s">
         <v>507</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="13" t="s">
         <v>506</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="13">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>793</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>794</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="13" t="s">
         <v>508</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="13">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>795</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="12" t="s">
         <v>796</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="12" t="s">
         <v>533</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="13" t="s">
         <v>510</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="13">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>797</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="12" t="s">
         <v>798</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="12" t="s">
         <v>534</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="13" t="s">
         <v>512</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="13" t="s">
         <v>513</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="13">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>799</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="12" t="s">
         <v>800</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="12" t="s">
         <v>535</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="13" t="s">
         <v>514</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="13" t="s">
         <v>515</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="13">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>801</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="12" t="s">
         <v>802</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="12" t="s">
         <v>536</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="13" t="s">
         <v>516</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="13" t="s">
         <v>517</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="13">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>803</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="12" t="s">
         <v>804</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="13">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>805</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="12" t="s">
         <v>806</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="13">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+    <row r="23" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>807</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="12" t="s">
         <v>808</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="12" t="s">
         <v>539</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="I23" s="16">
+      <c r="I23" s="13">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>809</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="12" t="s">
         <v>810</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="12" t="s">
         <v>540</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="13">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>811</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="12" t="s">
         <v>812</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="12" t="s">
         <v>541</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="13">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>813</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="12" t="s">
         <v>814</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="12" t="s">
         <v>542</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="13" t="s">
         <v>375</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="I26" s="16">
+      <c r="I26" s="13">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>815</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="12" t="s">
         <v>816</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="12" t="s">
         <v>543</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I27" s="13">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>817</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="12" t="s">
         <v>818</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="12" t="s">
         <v>544</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="13" t="s">
         <v>395</v>
       </c>
-      <c r="I28" s="16">
+      <c r="I28" s="13">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>819</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="12" t="s">
         <v>820</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="12" t="s">
         <v>545</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="13" t="s">
         <v>397</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H29" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="I29" s="16">
+      <c r="I29" s="13">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>821</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="12" t="s">
         <v>822</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="12" t="s">
         <v>546</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="G30" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="I30" s="16">
+      <c r="I30" s="13">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>823</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="12" t="s">
         <v>824</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="12" t="s">
         <v>547</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="13" t="s">
         <v>399</v>
       </c>
-      <c r="I31" s="16">
+      <c r="I31" s="13">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>825</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="12" t="s">
         <v>826</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="12" t="s">
         <v>548</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="13" t="s">
         <v>401</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="I32" s="16">
+      <c r="I32" s="13">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+    <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>827</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="12" t="s">
         <v>828</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="12" t="s">
         <v>549</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="13" t="s">
         <v>403</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="13" t="s">
         <v>404</v>
       </c>
-      <c r="I33" s="16">
+      <c r="I33" s="13">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>829</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="12" t="s">
         <v>830</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="I34" s="16">
+      <c r="I34" s="13">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+    <row r="35" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>831</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="12" t="s">
         <v>832</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="12" t="s">
         <v>551</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="I35" s="16">
+      <c r="I35" s="13">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+    <row r="36" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
         <v>833</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="12" t="s">
         <v>834</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="12" t="s">
         <v>552</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="F36" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="I36" s="16">
+      <c r="I36" s="13">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+    <row r="37" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
         <v>835</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="12" t="s">
         <v>836</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="12" t="s">
         <v>553</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G37" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H37" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="I37" s="16">
+      <c r="I37" s="13">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+    <row r="38" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>837</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="12" t="s">
         <v>838</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="12" t="s">
         <v>554</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="H38" s="16" t="s">
+      <c r="H38" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="I38" s="16">
+      <c r="I38" s="13">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
+    <row r="39" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>839</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="12" t="s">
         <v>840</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="12" t="s">
         <v>555</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E39" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="H39" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="I39" s="16">
+      <c r="I39" s="13">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+    <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>841</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="12" t="s">
         <v>842</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="12" t="s">
         <v>556</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="H40" s="16" t="s">
+      <c r="H40" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="I40" s="16">
+      <c r="I40" s="13">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+    <row r="41" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>843</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="12" t="s">
         <v>844</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="12" t="s">
         <v>557</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="I41" s="16">
+      <c r="I41" s="13">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
+    <row r="42" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>845</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="12" t="s">
         <v>846</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="13" t="s">
         <v>425</v>
       </c>
-      <c r="I42" s="16">
+      <c r="I42" s="13">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
+    <row r="43" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>847</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="12" t="s">
         <v>848</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="12" t="s">
         <v>559</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H43" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="I43" s="16">
+      <c r="I43" s="13">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+    <row r="44" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>849</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="12" t="s">
         <v>850</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="12" t="s">
         <v>560</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H44" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="I44" s="16">
+      <c r="I44" s="13">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
+    <row r="45" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>851</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="12" t="s">
         <v>852</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="12" t="s">
         <v>561</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="13" t="s">
         <v>432</v>
       </c>
-      <c r="I45" s="16">
+      <c r="I45" s="13">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+    <row r="46" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>853</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="12" t="s">
         <v>854</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H46" s="13" t="s">
         <v>434</v>
       </c>
-      <c r="I46" s="16">
+      <c r="I46" s="13">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
+    <row r="47" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>855</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="12" t="s">
         <v>856</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="13" t="s">
         <v>436</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H47" s="13" t="s">
         <v>435</v>
       </c>
-      <c r="I47" s="16">
+      <c r="I47" s="13">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+    <row r="48" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>857</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="12" t="s">
         <v>858</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="12" t="s">
         <v>564</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="F48" s="13" t="s">
         <v>439</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H48" s="13" t="s">
         <v>438</v>
       </c>
-      <c r="I48" s="16">
+      <c r="I48" s="13">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+    <row r="49" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>859</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="12" t="s">
         <v>860</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="12" t="s">
         <v>565</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="13" t="s">
         <v>441</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H49" s="13" t="s">
         <v>440</v>
       </c>
-      <c r="I49" s="16">
+      <c r="I49" s="13">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>861</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="12" t="s">
         <v>862</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="12" t="s">
         <v>566</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" s="13" t="s">
         <v>443</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="13" t="s">
         <v>444</v>
       </c>
-      <c r="I50" s="7">
+      <c r="I50" s="13">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>863</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="12" t="s">
         <v>864</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="13" t="s">
         <v>445</v>
       </c>
-      <c r="I51" s="7">
+      <c r="I51" s="13">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+    <row r="52" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
         <v>865</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="12" t="s">
         <v>866</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="13" t="s">
         <v>447</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="I52" s="7">
+      <c r="I52" s="13">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
         <v>867</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="12" t="s">
         <v>868</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="I53" s="7">
+      <c r="I53" s="13">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
         <v>869</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="12" t="s">
         <v>870</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="12" t="s">
         <v>570</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="I54" s="7">
+      <c r="I54" s="13">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
         <v>871</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="12" t="s">
         <v>872</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="12" t="s">
         <v>571</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="13" t="s">
         <v>453</v>
       </c>
-      <c r="I55" s="7">
+      <c r="I55" s="13">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
         <v>873</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="12" t="s">
         <v>874</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="12" t="s">
         <v>572</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="I56" s="7">
+      <c r="I56" s="13">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
         <v>875</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="12" t="s">
         <v>876</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="12" t="s">
         <v>573</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="I57" s="7">
+      <c r="I57" s="13">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+    <row r="58" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
         <v>877</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="12" t="s">
         <v>878</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="12" t="s">
         <v>574</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="13" t="s">
         <v>459</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="I58" s="7">
+      <c r="I58" s="13">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="12" t="s">
         <v>880</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="12" t="s">
         <v>575</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="I59" s="7">
+      <c r="I59" s="13">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
         <v>881</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="12" t="s">
         <v>882</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="12" t="s">
         <v>576</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="13" t="s">
         <v>463</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="I60" s="7">
+      <c r="I60" s="13">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
         <v>883</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="12" t="s">
         <v>884</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="12" t="s">
         <v>577</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="13" t="s">
         <v>465</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="13" t="s">
         <v>468</v>
       </c>
-      <c r="I61" s="7">
+      <c r="I61" s="13">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
         <v>885</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="12" t="s">
         <v>886</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="12" t="s">
         <v>578</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="I62" s="7">
+      <c r="I62" s="13">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
         <v>887</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="12" t="s">
         <v>888</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="12" t="s">
         <v>579</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="13" t="s">
         <v>469</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="13" t="s">
         <v>470</v>
       </c>
-      <c r="I63" s="7">
+      <c r="I63" s="13">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
         <v>889</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="12" t="s">
         <v>890</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="12" t="s">
         <v>580</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" s="13" t="s">
         <v>472</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="13" t="s">
         <v>471</v>
       </c>
-      <c r="I64" s="7">
+      <c r="I64" s="13">
         <v>63</v>
       </c>
     </row>
@@ -5898,72 +5893,72 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
+    <row r="69" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
         <v>899</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="12" t="s">
         <v>900</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="12" t="s">
         <v>585</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D69" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="F69" s="16" t="s">
+      <c r="F69" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H69" s="16" t="s">
+      <c r="H69" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="I69" s="16">
+      <c r="I69" s="13">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
+    <row r="70" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
         <v>901</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="12" t="s">
         <v>902</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C70" s="12" t="s">
         <v>586</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="D70" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="G70" s="16" t="s">
+      <c r="G70" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H70" s="16" t="s">
+      <c r="H70" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="I70" s="16">
+      <c r="I70" s="13">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
+    <row r="71" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
         <v>903</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="12" t="s">
         <v>904</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="12" t="s">
         <v>587</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="D71" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="F71" s="16" t="s">
+      <c r="F71" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="H71" s="16" t="s">
+      <c r="H71" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="I71" s="16">
+      <c r="I71" s="13">
         <v>70</v>
       </c>
     </row>
@@ -5990,26 +5985,26 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
+    <row r="73" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
         <v>907</v>
       </c>
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="12" t="s">
         <v>908</v>
       </c>
-      <c r="C73" s="15" t="s">
+      <c r="C73" s="12" t="s">
         <v>589</v>
       </c>
-      <c r="D73" s="16" t="s">
+      <c r="D73" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G73" s="16" t="s">
+      <c r="G73" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H73" s="16" t="s">
+      <c r="H73" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I73" s="16">
+      <c r="I73" s="13">
         <v>72</v>
       </c>
     </row>
@@ -6036,26 +6031,26 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14" t="s">
+    <row r="75" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
         <v>911</v>
       </c>
-      <c r="B75" s="15" t="s">
+      <c r="B75" s="12" t="s">
         <v>912</v>
       </c>
-      <c r="C75" s="15" t="s">
+      <c r="C75" s="12" t="s">
         <v>591</v>
       </c>
-      <c r="D75" s="16" t="s">
+      <c r="D75" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E75" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H75" s="16" t="s">
+      <c r="H75" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="I75" s="16">
+      <c r="I75" s="13">
         <v>74</v>
       </c>
     </row>
@@ -6082,601 +6077,601 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14" t="s">
+    <row r="77" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
         <v>915</v>
       </c>
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="12" t="s">
         <v>916</v>
       </c>
-      <c r="C77" s="15" t="s">
+      <c r="C77" s="12" t="s">
         <v>593</v>
       </c>
-      <c r="D77" s="16" t="s">
+      <c r="D77" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="E77" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H77" s="16" t="s">
+      <c r="H77" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I77" s="16">
+      <c r="I77" s="13">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
+    <row r="78" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="12" t="s">
         <v>918</v>
       </c>
-      <c r="C78" s="15" t="s">
+      <c r="C78" s="12" t="s">
         <v>594</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="D78" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E78" s="16" t="s">
+      <c r="E78" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H78" s="16" t="s">
+      <c r="H78" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I78" s="16">
+      <c r="I78" s="13">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
+    <row r="79" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
         <v>919</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="B79" s="12" t="s">
         <v>920</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="C79" s="12" t="s">
         <v>595</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="D79" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="E79" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H79" s="16" t="s">
+      <c r="H79" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I79" s="16">
+      <c r="I79" s="13">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+    <row r="80" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
         <v>921</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="12" t="s">
         <v>922</v>
       </c>
-      <c r="C80" s="15" t="s">
+      <c r="C80" s="12" t="s">
         <v>596</v>
       </c>
-      <c r="D80" s="16" t="s">
+      <c r="D80" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E80" s="16" t="s">
+      <c r="E80" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H80" s="16" t="s">
+      <c r="H80" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I80" s="16">
+      <c r="I80" s="13">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
+    <row r="81" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
         <v>923</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="12" t="s">
         <v>924</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="C81" s="12" t="s">
         <v>597</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F81" s="16" t="s">
+      <c r="F81" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H81" s="16" t="s">
+      <c r="H81" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I81" s="16">
+      <c r="I81" s="13">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
+    <row r="82" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
         <v>925</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="12" t="s">
         <v>926</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="12" t="s">
         <v>598</v>
       </c>
-      <c r="D82" s="16" t="s">
+      <c r="D82" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F82" s="16" t="s">
+      <c r="F82" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H82" s="16" t="s">
+      <c r="H82" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="I82" s="16">
+      <c r="I82" s="13">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
+    <row r="83" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
         <v>927</v>
       </c>
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="12" t="s">
         <v>928</v>
       </c>
-      <c r="C83" s="15" t="s">
+      <c r="C83" s="12" t="s">
         <v>599</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="D83" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F83" s="16" t="s">
+      <c r="F83" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="H83" s="16" t="s">
+      <c r="H83" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I83" s="16">
+      <c r="I83" s="13">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
+    <row r="84" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
         <v>929</v>
       </c>
-      <c r="B84" s="15" t="s">
+      <c r="B84" s="12" t="s">
         <v>930</v>
       </c>
-      <c r="C84" s="15" t="s">
+      <c r="C84" s="12" t="s">
         <v>600</v>
       </c>
-      <c r="D84" s="16" t="s">
+      <c r="D84" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G84" s="16" t="s">
+      <c r="G84" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="H84" s="16" t="s">
+      <c r="H84" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I84" s="16">
+      <c r="I84" s="13">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14" t="s">
+    <row r="85" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
         <v>931</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="12" t="s">
         <v>932</v>
       </c>
-      <c r="C85" s="15" t="s">
+      <c r="C85" s="12" t="s">
         <v>601</v>
       </c>
-      <c r="D85" s="16" t="s">
+      <c r="D85" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F85" s="16" t="s">
+      <c r="F85" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H85" s="16" t="s">
+      <c r="H85" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="I85" s="16">
+      <c r="I85" s="13">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14" t="s">
+    <row r="86" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
         <v>933</v>
       </c>
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="12" t="s">
         <v>934</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="12" t="s">
         <v>602</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="D86" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F86" s="16" t="s">
+      <c r="F86" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H86" s="16" t="s">
+      <c r="H86" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I86" s="16">
+      <c r="I86" s="13">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="s">
+    <row r="87" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
         <v>935</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B87" s="12" t="s">
         <v>936</v>
       </c>
-      <c r="C87" s="15" t="s">
+      <c r="C87" s="12" t="s">
         <v>603</v>
       </c>
-      <c r="D87" s="16" t="s">
+      <c r="D87" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F87" s="16" t="s">
+      <c r="F87" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="H87" s="16" t="s">
+      <c r="H87" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I87" s="16">
+      <c r="I87" s="13">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="s">
+    <row r="88" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
         <v>937</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="12" t="s">
         <v>938</v>
       </c>
-      <c r="C88" s="15" t="s">
+      <c r="C88" s="12" t="s">
         <v>604</v>
       </c>
-      <c r="D88" s="16" t="s">
+      <c r="D88" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F88" s="16" t="s">
+      <c r="F88" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H88" s="16" t="s">
+      <c r="H88" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="I88" s="16">
+      <c r="I88" s="13">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14" t="s">
+    <row r="89" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
         <v>939</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="12" t="s">
         <v>940</v>
       </c>
-      <c r="C89" s="15" t="s">
+      <c r="C89" s="12" t="s">
         <v>605</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D89" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F89" s="16" t="s">
+      <c r="F89" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H89" s="16" t="s">
+      <c r="H89" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I89" s="16">
+      <c r="I89" s="13">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14" t="s">
+    <row r="90" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
         <v>941</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B90" s="12" t="s">
         <v>942</v>
       </c>
-      <c r="C90" s="15" t="s">
+      <c r="C90" s="12" t="s">
         <v>606</v>
       </c>
-      <c r="D90" s="16" t="s">
+      <c r="D90" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E90" s="16" t="s">
+      <c r="E90" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H90" s="16" t="s">
+      <c r="H90" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I90" s="16">
+      <c r="I90" s="13">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14" t="s">
+    <row r="91" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
         <v>943</v>
       </c>
-      <c r="B91" s="15" t="s">
+      <c r="B91" s="12" t="s">
         <v>944</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C91" s="12" t="s">
         <v>607</v>
       </c>
-      <c r="D91" s="16" t="s">
+      <c r="D91" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E91" s="16" t="s">
+      <c r="E91" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H91" s="16" t="s">
+      <c r="H91" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="I91" s="16">
+      <c r="I91" s="13">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14" t="s">
+    <row r="92" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
         <v>945</v>
       </c>
-      <c r="B92" s="15" t="s">
+      <c r="B92" s="12" t="s">
         <v>946</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="C92" s="12" t="s">
         <v>608</v>
       </c>
-      <c r="D92" s="16" t="s">
+      <c r="D92" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E92" s="16" t="s">
+      <c r="E92" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H92" s="16" t="s">
+      <c r="H92" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="I92" s="16">
+      <c r="I92" s="13">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="14" t="s">
+    <row r="93" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
         <v>947</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="12" t="s">
         <v>948</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="C93" s="12" t="s">
         <v>609</v>
       </c>
-      <c r="D93" s="16" t="s">
+      <c r="D93" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="E93" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="H93" s="16" t="s">
+      <c r="H93" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="I93" s="16">
+      <c r="I93" s="13">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="s">
+    <row r="94" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
         <v>949</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="12" t="s">
         <v>950</v>
       </c>
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="12" t="s">
         <v>610</v>
       </c>
-      <c r="D94" s="16" t="s">
+      <c r="D94" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="E94" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H94" s="16" t="s">
+      <c r="H94" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I94" s="16">
+      <c r="I94" s="13">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14" t="s">
+    <row r="95" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
         <v>951</v>
       </c>
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="12" t="s">
         <v>952</v>
       </c>
-      <c r="C95" s="15" t="s">
+      <c r="C95" s="12" t="s">
         <v>611</v>
       </c>
-      <c r="D95" s="16" t="s">
+      <c r="D95" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="E95" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H95" s="16" t="s">
+      <c r="H95" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="I95" s="16">
+      <c r="I95" s="13">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14" t="s">
+    <row r="96" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
         <v>953</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="12" t="s">
         <v>954</v>
       </c>
-      <c r="C96" s="15" t="s">
+      <c r="C96" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="D96" s="16" t="s">
+      <c r="D96" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E96" s="16" t="s">
+      <c r="E96" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="H96" s="16" t="s">
+      <c r="H96" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="I96" s="16">
+      <c r="I96" s="13">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
+    <row r="97" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
         <v>955</v>
       </c>
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="12" t="s">
         <v>956</v>
       </c>
-      <c r="C97" s="15" t="s">
+      <c r="C97" s="12" t="s">
         <v>613</v>
       </c>
-      <c r="D97" s="16" t="s">
+      <c r="D97" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="E97" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H97" s="16" t="s">
+      <c r="H97" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I97" s="16">
+      <c r="I97" s="13">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14" t="s">
+    <row r="98" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
         <v>957</v>
       </c>
-      <c r="B98" s="15" t="s">
+      <c r="B98" s="12" t="s">
         <v>958</v>
       </c>
-      <c r="C98" s="15" t="s">
+      <c r="C98" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="D98" s="16" t="s">
+      <c r="D98" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="E98" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H98" s="16" t="s">
+      <c r="H98" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="I98" s="16">
+      <c r="I98" s="13">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14" t="s">
+    <row r="99" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
         <v>959</v>
       </c>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="12" t="s">
         <v>960</v>
       </c>
-      <c r="C99" s="15" t="s">
+      <c r="C99" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="D99" s="16" t="s">
+      <c r="D99" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E99" s="16" t="s">
+      <c r="E99" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H99" s="16" t="s">
+      <c r="H99" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I99" s="16">
+      <c r="I99" s="13">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14" t="s">
+    <row r="100" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
         <v>961</v>
       </c>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="12" t="s">
         <v>962</v>
       </c>
-      <c r="C100" s="15" t="s">
+      <c r="C100" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="D100" s="16" t="s">
+      <c r="D100" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E100" s="16" t="s">
+      <c r="E100" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H100" s="16" t="s">
+      <c r="H100" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="I100" s="16">
+      <c r="I100" s="13">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="14" t="s">
+    <row r="101" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="11" t="s">
         <v>963</v>
       </c>
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="12" t="s">
         <v>964</v>
       </c>
-      <c r="C101" s="15" t="s">
+      <c r="C101" s="12" t="s">
         <v>617</v>
       </c>
-      <c r="D101" s="16" t="s">
+      <c r="D101" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E101" s="16" t="s">
+      <c r="E101" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="H101" s="16" t="s">
+      <c r="H101" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="I101" s="16">
+      <c r="I101" s="13">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14" t="s">
+    <row r="102" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="11" t="s">
         <v>965</v>
       </c>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="12" t="s">
         <v>966</v>
       </c>
-      <c r="C102" s="15" t="s">
+      <c r="C102" s="12" t="s">
         <v>618</v>
       </c>
-      <c r="D102" s="16" t="s">
+      <c r="D102" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G102" s="16" t="s">
+      <c r="G102" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="H102" s="16" t="s">
+      <c r="H102" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="I102" s="16">
+      <c r="I102" s="13">
         <v>101</v>
       </c>
     </row>
@@ -6703,72 +6698,72 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14" t="s">
+    <row r="104" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
         <v>969</v>
       </c>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="12" t="s">
         <v>970</v>
       </c>
-      <c r="C104" s="15" t="s">
+      <c r="C104" s="12" t="s">
         <v>620</v>
       </c>
-      <c r="D104" s="16" t="s">
+      <c r="D104" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F104" s="16" t="s">
+      <c r="F104" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="H104" s="16" t="s">
+      <c r="H104" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="I104" s="16">
+      <c r="I104" s="13">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14" t="s">
+    <row r="105" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="11" t="s">
         <v>971</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="12" t="s">
         <v>972</v>
       </c>
-      <c r="C105" s="15" t="s">
+      <c r="C105" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="D105" s="16" t="s">
+      <c r="D105" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F105" s="16" t="s">
+      <c r="F105" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="H105" s="16" t="s">
+      <c r="H105" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="I105" s="16">
+      <c r="I105" s="13">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14" t="s">
+    <row r="106" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
         <v>973</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B106" s="12" t="s">
         <v>974</v>
       </c>
-      <c r="C106" s="15" t="s">
+      <c r="C106" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="D106" s="16" t="s">
+      <c r="D106" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F106" s="16" t="s">
+      <c r="F106" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H106" s="16" t="s">
+      <c r="H106" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="I106" s="16">
+      <c r="I106" s="13">
         <v>105</v>
       </c>
     </row>
@@ -6795,26 +6790,26 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="14" t="s">
+    <row r="108" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="11" t="s">
         <v>977</v>
       </c>
-      <c r="B108" s="15" t="s">
+      <c r="B108" s="12" t="s">
         <v>978</v>
       </c>
-      <c r="C108" s="15" t="s">
+      <c r="C108" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="D108" s="16" t="s">
+      <c r="D108" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F108" s="16" t="s">
+      <c r="F108" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="H108" s="16" t="s">
+      <c r="H108" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I108" s="16">
+      <c r="I108" s="13">
         <v>107</v>
       </c>
     </row>
@@ -6841,26 +6836,26 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
+    <row r="110" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="11" t="s">
         <v>981</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="12" t="s">
         <v>982</v>
       </c>
-      <c r="C110" s="15" t="s">
+      <c r="C110" s="12" t="s">
         <v>626</v>
       </c>
-      <c r="D110" s="16" t="s">
+      <c r="D110" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F110" s="16" t="s">
+      <c r="F110" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="H110" s="16" t="s">
+      <c r="H110" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="I110" s="16">
+      <c r="I110" s="13">
         <v>109</v>
       </c>
     </row>
@@ -6887,49 +6882,49 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="14" t="s">
+    <row r="112" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="11" t="s">
         <v>985</v>
       </c>
-      <c r="B112" s="15" t="s">
+      <c r="B112" s="12" t="s">
         <v>986</v>
       </c>
-      <c r="C112" s="15" t="s">
+      <c r="C112" s="12" t="s">
         <v>628</v>
       </c>
-      <c r="D112" s="16" t="s">
+      <c r="D112" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F112" s="16" t="s">
+      <c r="F112" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="H112" s="16" t="s">
+      <c r="H112" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="I112" s="16">
+      <c r="I112" s="13">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="s">
+    <row r="113" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="11" t="s">
         <v>987</v>
       </c>
-      <c r="B113" s="15" t="s">
+      <c r="B113" s="12" t="s">
         <v>988</v>
       </c>
-      <c r="C113" s="15" t="s">
+      <c r="C113" s="12" t="s">
         <v>629</v>
       </c>
-      <c r="D113" s="16" t="s">
+      <c r="D113" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F113" s="16" t="s">
+      <c r="F113" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H113" s="16" t="s">
+      <c r="H113" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I113" s="16">
+      <c r="I113" s="13">
         <v>112</v>
       </c>
     </row>
@@ -7002,164 +6997,164 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="s">
+    <row r="117" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="11" t="s">
         <v>995</v>
       </c>
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="12" t="s">
         <v>996</v>
       </c>
-      <c r="C117" s="15" t="s">
+      <c r="C117" s="12" t="s">
         <v>633</v>
       </c>
-      <c r="D117" s="16" t="s">
+      <c r="D117" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G117" s="16" t="s">
+      <c r="G117" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H117" s="16" t="s">
+      <c r="H117" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="I117" s="16">
+      <c r="I117" s="13">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14" t="s">
+    <row r="118" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="11" t="s">
         <v>997</v>
       </c>
-      <c r="B118" s="15" t="s">
+      <c r="B118" s="12" t="s">
         <v>998</v>
       </c>
-      <c r="C118" s="15" t="s">
+      <c r="C118" s="12" t="s">
         <v>634</v>
       </c>
-      <c r="D118" s="16" t="s">
+      <c r="D118" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G118" s="16" t="s">
+      <c r="G118" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H118" s="16" t="s">
+      <c r="H118" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I118" s="16">
+      <c r="I118" s="13">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="s">
+    <row r="119" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="11" t="s">
         <v>999</v>
       </c>
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="12" t="s">
         <v>1000</v>
       </c>
-      <c r="C119" s="15" t="s">
+      <c r="C119" s="12" t="s">
         <v>635</v>
       </c>
-      <c r="D119" s="16" t="s">
+      <c r="D119" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G119" s="16" t="s">
+      <c r="G119" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H119" s="16" t="s">
+      <c r="H119" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I119" s="16">
+      <c r="I119" s="13">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
+    <row r="120" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="11" t="s">
         <v>1001</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="12" t="s">
         <v>1002</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C120" s="12" t="s">
         <v>636</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G120" t="s">
+      <c r="G120" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H120" t="s">
+      <c r="H120" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I120" s="7">
+      <c r="I120" s="13">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="4" t="s">
+    <row r="121" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
         <v>1003</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="12" t="s">
         <v>1004</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C121" s="12" t="s">
         <v>637</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G121" t="s">
+      <c r="G121" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H121" t="s">
+      <c r="H121" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I121" s="7">
+      <c r="I121" s="13">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
+    <row r="122" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="11" t="s">
         <v>1005</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="12" t="s">
         <v>1006</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C122" s="12" t="s">
         <v>638</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G122" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H122" t="s">
+      <c r="H122" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I122" s="7">
+      <c r="I122" s="13">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
+    <row r="123" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="11" t="s">
         <v>1007</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="12" t="s">
         <v>1008</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="C123" s="12" t="s">
         <v>639</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G123" t="s">
+      <c r="G123" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H123" t="s">
+      <c r="H123" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I123" s="7">
+      <c r="I123" s="13">
         <v>122</v>
       </c>
     </row>
@@ -7186,256 +7181,256 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
+    <row r="125" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="11" t="s">
         <v>1011</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="12" t="s">
         <v>1012</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="C125" s="12" t="s">
         <v>641</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G125" t="s">
+      <c r="G125" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H125" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I125" s="7">
+      <c r="I125" s="13">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
+    <row r="126" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="11" t="s">
         <v>1013</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B126" s="12" t="s">
         <v>1014</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="C126" s="12" t="s">
         <v>642</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G126" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H126" t="s">
+      <c r="H126" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I126" s="7">
+      <c r="I126" s="13">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
+    <row r="127" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="11" t="s">
         <v>1015</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B127" s="12" t="s">
         <v>1016</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="12" t="s">
         <v>643</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G127" t="s">
+      <c r="G127" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H127" t="s">
+      <c r="H127" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I127" s="7">
+      <c r="I127" s="13">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="4" t="s">
+    <row r="128" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="11" t="s">
         <v>1017</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" s="12" t="s">
         <v>1018</v>
       </c>
-      <c r="C128" s="3" t="s">
+      <c r="C128" s="12" t="s">
         <v>644</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G128" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H128" t="s">
+      <c r="H128" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I128" s="7">
+      <c r="I128" s="13">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="4" t="s">
+    <row r="129" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="11" t="s">
         <v>1019</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B129" s="12" t="s">
         <v>1020</v>
       </c>
-      <c r="C129" s="3" t="s">
+      <c r="C129" s="12" t="s">
         <v>645</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G129" t="s">
+      <c r="G129" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H129" t="s">
+      <c r="H129" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I129" s="7">
+      <c r="I129" s="13">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="4" t="s">
+    <row r="130" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="11" t="s">
         <v>1021</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B130" s="12" t="s">
         <v>1022</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C130" s="12" t="s">
         <v>646</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G130" t="s">
+      <c r="G130" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H130" t="s">
+      <c r="H130" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I130" s="7">
+      <c r="I130" s="13">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
+    <row r="131" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="11" t="s">
         <v>1023</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="B131" s="12" t="s">
         <v>1024</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="C131" s="12" t="s">
         <v>647</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G131" t="s">
+      <c r="G131" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H131" t="s">
+      <c r="H131" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I131" s="7">
+      <c r="I131" s="13">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
+    <row r="132" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="11" t="s">
         <v>1025</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B132" s="12" t="s">
         <v>1026</v>
       </c>
-      <c r="C132" s="3" t="s">
+      <c r="C132" s="12" t="s">
         <v>648</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G132" t="s">
+      <c r="G132" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H132" t="s">
+      <c r="H132" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I132" s="7">
+      <c r="I132" s="13">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="4" t="s">
+    <row r="133" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="11" t="s">
         <v>1027</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B133" s="12" t="s">
         <v>1028</v>
       </c>
-      <c r="C133" s="3" t="s">
+      <c r="C133" s="12" t="s">
         <v>649</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G133" t="s">
+      <c r="G133" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H133" t="s">
+      <c r="H133" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I133" s="7">
+      <c r="I133" s="13">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="4" t="s">
+    <row r="134" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="11" t="s">
         <v>1029</v>
       </c>
-      <c r="B134" s="3" t="s">
+      <c r="B134" s="12" t="s">
         <v>1030</v>
       </c>
-      <c r="C134" s="3" t="s">
+      <c r="C134" s="12" t="s">
         <v>650</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G134" t="s">
+      <c r="G134" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H134" t="s">
+      <c r="H134" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I134" s="7">
+      <c r="I134" s="13">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="4" t="s">
+    <row r="135" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="11" t="s">
         <v>1031</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="B135" s="12" t="s">
         <v>1032</v>
       </c>
-      <c r="C135" s="3" t="s">
+      <c r="C135" s="12" t="s">
         <v>651</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G135" t="s">
+      <c r="G135" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H135" t="s">
+      <c r="H135" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I135" s="7">
+      <c r="I135" s="13">
         <v>134</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambio de Char set
</commit_message>
<xml_diff>
--- a/Videos (1).xlsx
+++ b/Videos (1).xlsx
@@ -4296,7 +4296,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4306,8 +4306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200:XFD200"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A233" sqref="A233:XFD233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8860,49 +8860,49 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A198" s="4" t="s">
+    <row r="198" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="11" t="s">
         <v>1157</v>
       </c>
-      <c r="B198" s="3" t="s">
+      <c r="B198" s="12" t="s">
         <v>1158</v>
       </c>
-      <c r="C198" s="3" t="s">
+      <c r="C198" s="12" t="s">
         <v>714</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E198" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="H198" t="s">
+      <c r="H198" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="I198" s="7">
+      <c r="I198" s="13">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A199" s="4" t="s">
+    <row r="199" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="11" t="s">
         <v>1159</v>
       </c>
-      <c r="B199" s="3" t="s">
+      <c r="B199" s="12" t="s">
         <v>1160</v>
       </c>
-      <c r="C199" s="3" t="s">
+      <c r="C199" s="12" t="s">
         <v>715</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="E199" t="s">
+      <c r="E199" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="H199" t="s">
+      <c r="H199" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="I199" s="7">
+      <c r="I199" s="13">
         <v>198</v>
       </c>
     </row>
@@ -9366,72 +9366,72 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A220" s="4" t="s">
+    <row r="220" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="11" t="s">
         <v>1201</v>
       </c>
-      <c r="B220" s="3" t="s">
+      <c r="B220" s="12" t="s">
         <v>1202</v>
       </c>
-      <c r="C220" s="3" t="s">
+      <c r="C220" s="12" t="s">
         <v>736</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E220" t="s">
+      <c r="E220" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="H220" t="s">
+      <c r="H220" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="I220" s="7">
+      <c r="I220" s="13">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A221" s="4" t="s">
+    <row r="221" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="11" t="s">
         <v>1203</v>
       </c>
-      <c r="B221" s="3" t="s">
+      <c r="B221" s="12" t="s">
         <v>1204</v>
       </c>
-      <c r="C221" s="3" t="s">
+      <c r="C221" s="12" t="s">
         <v>737</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E221" t="s">
+      <c r="E221" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="H221" t="s">
+      <c r="H221" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="I221" s="7">
+      <c r="I221" s="13">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A222" s="4" t="s">
+    <row r="222" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="11" t="s">
         <v>1205</v>
       </c>
-      <c r="B222" s="3" t="s">
+      <c r="B222" s="12" t="s">
         <v>1206</v>
       </c>
-      <c r="C222" s="3" t="s">
+      <c r="C222" s="12" t="s">
         <v>738</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="H222" t="s">
+      <c r="H222" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="I222" s="7">
+      <c r="I222" s="13">
         <v>221</v>
       </c>
     </row>
@@ -9527,72 +9527,72 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A227" s="4" t="s">
+    <row r="227" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="11" t="s">
         <v>1215</v>
       </c>
-      <c r="B227" s="3" t="s">
+      <c r="B227" s="12" t="s">
         <v>1216</v>
       </c>
-      <c r="C227" s="3" t="s">
+      <c r="C227" s="12" t="s">
         <v>743</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E227" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="H227" t="s">
+      <c r="H227" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="I227" s="7">
+      <c r="I227" s="13">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A228" s="4" t="s">
+    <row r="228" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="11" t="s">
         <v>1217</v>
       </c>
-      <c r="B228" s="3" t="s">
+      <c r="B228" s="12" t="s">
         <v>1218</v>
       </c>
-      <c r="C228" s="3" t="s">
+      <c r="C228" s="12" t="s">
         <v>744</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E228" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="H228" t="s">
+      <c r="H228" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="I228" s="7">
+      <c r="I228" s="13">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A229" s="4" t="s">
+    <row r="229" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="11" t="s">
         <v>1219</v>
       </c>
-      <c r="B229" s="3" t="s">
+      <c r="B229" s="12" t="s">
         <v>1220</v>
       </c>
-      <c r="C229" s="3" t="s">
+      <c r="C229" s="12" t="s">
         <v>745</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E229" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H229" t="s">
+      <c r="H229" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="I229" s="7">
+      <c r="I229" s="13">
         <v>228</v>
       </c>
     </row>
@@ -9665,49 +9665,49 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A233" s="4" t="s">
+    <row r="233" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="11" t="s">
         <v>1227</v>
       </c>
-      <c r="B233" s="3" t="s">
+      <c r="B233" s="12" t="s">
         <v>1228</v>
       </c>
-      <c r="C233" s="3" t="s">
+      <c r="C233" s="12" t="s">
         <v>749</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E233" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="H233" t="s">
+      <c r="H233" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="I233" s="7">
+      <c r="I233" s="13">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A234" s="4" t="s">
+    <row r="234" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="11" t="s">
         <v>1229</v>
       </c>
-      <c r="B234" s="3" t="s">
+      <c r="B234" s="12" t="s">
         <v>1230</v>
       </c>
-      <c r="C234" s="3" t="s">
+      <c r="C234" s="12" t="s">
         <v>750</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E234" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="H234" t="s">
+      <c r="H234" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="I234" s="7">
+      <c r="I234" s="13">
         <v>233</v>
       </c>
     </row>
@@ -9734,72 +9734,72 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A236" s="4" t="s">
+    <row r="236" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="11" t="s">
         <v>1233</v>
       </c>
-      <c r="B236" s="3" t="s">
+      <c r="B236" s="12" t="s">
         <v>1234</v>
       </c>
-      <c r="C236" s="3" t="s">
+      <c r="C236" s="12" t="s">
         <v>752</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="E236" t="s">
+      <c r="E236" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="H236" t="s">
+      <c r="H236" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="I236" s="7">
+      <c r="I236" s="13">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A237" s="4" t="s">
+    <row r="237" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="11" t="s">
         <v>1235</v>
       </c>
-      <c r="B237" s="3" t="s">
+      <c r="B237" s="12" t="s">
         <v>1236</v>
       </c>
-      <c r="C237" s="3" t="s">
+      <c r="C237" s="12" t="s">
         <v>753</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E237" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="H237" t="s">
+      <c r="H237" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="I237" s="7">
+      <c r="I237" s="13">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A238" s="4" t="s">
+    <row r="238" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="11" t="s">
         <v>1237</v>
       </c>
-      <c r="B238" s="3" t="s">
+      <c r="B238" s="12" t="s">
         <v>1238</v>
       </c>
-      <c r="C238" s="3" t="s">
+      <c r="C238" s="12" t="s">
         <v>754</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E238" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="H238" t="s">
+      <c r="H238" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="I238" s="7">
+      <c r="I238" s="13">
         <v>237</v>
       </c>
     </row>

</xml_diff>